<commit_message>
corrected learning start year
</commit_message>
<xml_diff>
--- a/inputs/component_inputs.xlsx
+++ b/inputs/component_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyoung\Documents\GitHub\hydrogen-optimisation-research\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB27A7B2-649B-40A1-8829-B187BD94D234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F6345C-205C-4DFA-8075-B0896F392C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{87E1AC9F-C52D-46BE-BFA9-EAAC32F5E6CD}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="8" xr2:uid="{87E1AC9F-C52D-46BE-BFA9-EAAC32F5E6CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Economic Inputs" sheetId="14" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>Simplify Efficiencies to Five Points</t>
   </si>
   <si>
-    <t>Capital Cost Baseline Year</t>
-  </si>
-  <si>
     <t>Capital Cost Price Year</t>
   </si>
   <si>
@@ -314,9 +311,6 @@
   </si>
   <si>
     <t>Combined Electricity Price Inflation</t>
-  </si>
-  <si>
-    <t>The year for which the capital costs are estimated</t>
   </si>
   <si>
     <t>The price year for which the capital costs are quoted</t>
@@ -366,6 +360,12 @@
   </si>
   <si>
     <t>To account for any losses between metering point and electrolyser</t>
+  </si>
+  <si>
+    <t>Component Delivery Year</t>
+  </si>
+  <si>
+    <t>The input capital costs must relate to delivery in this year</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" customHeight="1"/>
@@ -1087,46 +1087,46 @@
     </row>
     <row r="2" spans="1:3" ht="19.2" customHeight="1">
       <c r="A2" s="51" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B2" s="52">
         <v>2025</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.2" customHeight="1">
       <c r="A3" s="51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="52">
         <v>2023</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.2" customHeight="1">
       <c r="A4" s="51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="52">
         <v>2022</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.2" customHeight="1">
       <c r="A5" s="51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="55">
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.2" customHeight="1">
@@ -1166,7 +1166,7 @@
     </row>
     <row r="10" spans="1:3" ht="19.2" customHeight="1">
       <c r="A10" s="51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B10" s="52">
         <v>46.1</v>
@@ -1174,7 +1174,7 @@
     </row>
     <row r="11" spans="1:3" ht="19.2" customHeight="1">
       <c r="A11" s="51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B11" s="52">
         <v>569</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="15" spans="1:3" ht="19.2" customHeight="1">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" s="52">
         <v>0.62</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="16" spans="1:3" ht="19.2" customHeight="1">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" s="52">
         <v>4.46</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="17" spans="1:3" ht="19.2" customHeight="1">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B17" s="52">
         <v>0.39</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="18" spans="1:3" ht="19.2" customHeight="1">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B18" s="52">
         <v>0.16</v>
@@ -1238,14 +1238,14 @@
     </row>
     <row r="19" spans="1:3" ht="19.2" customHeight="1">
       <c r="A19" s="58" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B19" s="59">
         <f>SUM(B15:B18)</f>
         <v>5.63</v>
       </c>
       <c r="C19" s="52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -10560,7 +10560,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" customHeight="1"/>
@@ -10605,7 +10605,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.2" customHeight="1">
@@ -10663,7 +10663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876A8463-2B96-461E-9F1D-83F4C3412B20}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -47007,7 +47007,7 @@
   <dimension ref="A1:Z974"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="14.4"/>
@@ -47483,10 +47483,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="45">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" s="39" t="s">
         <v>61</v>
@@ -48500,7 +48500,7 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New batch file downloads added
</commit_message>
<xml_diff>
--- a/inputs/component_inputs.xlsx
+++ b/inputs/component_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyoung\Documents\GitHub\hydrogen-optimisation-research\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EBE375-B3A3-495E-BFD4-CBF652E5BBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F998BFD3-3255-4047-923F-F907C1C84562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{87E1AC9F-C52D-46BE-BFA9-EAAC32F5E6CD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{87E1AC9F-C52D-46BE-BFA9-EAAC32F5E6CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Economic Inputs" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
   <si>
     <t>id</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>The input capital costs must relate to delivery in this year</t>
+  </si>
+  <si>
+    <t>If run in batch mode, the N best setups will have their detailed results downloaded. N is equal to the value given here.</t>
+  </si>
+  <si>
+    <t>Number of Batch Setups to Download</t>
   </si>
 </sst>
 </file>
@@ -1067,14 +1073,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.149999999999999" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="19.2" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" style="51" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="52"/>
-    <col min="3" max="3" width="135.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" style="51" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="52"/>
+    <col min="3" max="3" width="135.44140625" style="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="1" spans="1:3" ht="19.2" customHeight="1">
       <c r="A1" s="49" t="s">
         <v>68</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="2" spans="1:3" ht="19.2" customHeight="1">
       <c r="A2" s="51" t="s">
         <v>99</v>
       </c>
@@ -1096,7 +1102,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="3" spans="1:3" ht="19.2" customHeight="1">
       <c r="A3" s="51" t="s">
         <v>84</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="4" spans="1:3" ht="19.2" customHeight="1">
       <c r="A4" s="51" t="s">
         <v>85</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="5" spans="1:3" ht="19.2" customHeight="1">
       <c r="A5" s="51" t="s">
         <v>86</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="6" spans="1:3" ht="19.2" customHeight="1">
       <c r="A6" s="51" t="s">
         <v>63</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="7" spans="1:3" ht="19.2" customHeight="1">
       <c r="A7" s="53" t="s">
         <v>64</v>
       </c>
@@ -1145,7 +1151,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="8" spans="1:3" ht="19.2" customHeight="1">
       <c r="A8" s="51" t="s">
         <v>65</v>
       </c>
@@ -1153,7 +1159,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="9" spans="1:3" ht="19.2" customHeight="1">
       <c r="A9" s="51" t="s">
         <v>66</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="10" spans="1:3" ht="19.2" customHeight="1">
       <c r="A10" s="51" t="s">
         <v>97</v>
       </c>
@@ -1172,7 +1178,7 @@
         <v>46.1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="11" spans="1:3" ht="19.2" customHeight="1">
       <c r="A11" s="51" t="s">
         <v>96</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="12" spans="1:3" ht="19.2" customHeight="1">
       <c r="A12" s="51" t="s">
         <v>72</v>
       </c>
@@ -1188,7 +1194,7 @@
         <v>601.76</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="13" spans="1:3" ht="19.2" customHeight="1">
       <c r="A13" s="51" t="s">
         <v>73</v>
       </c>
@@ -1196,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="14" spans="1:3" ht="19.2" customHeight="1">
       <c r="A14" s="51" t="s">
         <v>74</v>
       </c>
@@ -1204,7 +1210,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="15" spans="1:3" ht="19.2" customHeight="1">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1212,7 +1218,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="16" spans="1:3" ht="19.2" customHeight="1">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>4.46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="17" spans="1:3" ht="19.2" customHeight="1">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="18" spans="1:3" ht="19.2" customHeight="1">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -1236,7 +1242,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="19" spans="1:3" ht="19.2" customHeight="1">
       <c r="A19" s="58" t="s">
         <v>94</v>
       </c>
@@ -1265,15 +1271,15 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="12.5703125" style="5"/>
+    <col min="5" max="5" width="14.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="12.5546875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
@@ -5672,14 +5678,14 @@
       <selection activeCell="D8" sqref="D8:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="5"/>
+    <col min="1" max="1" width="12.5546875" style="5"/>
     <col min="2" max="2" width="20" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="5"/>
-    <col min="5" max="5" width="13.28515625" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="5"/>
+    <col min="3" max="3" width="22.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="5"/>
+    <col min="5" max="5" width="13.33203125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="12.5546875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
@@ -9858,14 +9864,14 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="5"/>
+    <col min="4" max="4" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.5546875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -10557,20 +10563,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EBA260-5F35-4402-8789-C2ABB030CA84}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.149999999999999" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="19.2" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="54"/>
-    <col min="3" max="3" width="31.28515625" style="52" customWidth="1"/>
+    <col min="1" max="1" width="50.77734375" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="54"/>
+    <col min="3" max="3" width="37.6640625" style="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="1" spans="1:3" ht="19.2" customHeight="1">
       <c r="A1" s="49" t="s">
         <v>68</v>
       </c>
@@ -10581,7 +10587,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="2" spans="1:3" ht="19.2" customHeight="1">
       <c r="A2" s="51" t="s">
         <v>75</v>
       </c>
@@ -10589,7 +10595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="3" spans="1:3" ht="19.2" customHeight="1">
       <c r="A3" s="53" t="s">
         <v>76</v>
       </c>
@@ -10608,7 +10614,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="5" spans="1:3" ht="19.2" customHeight="1">
       <c r="A5" s="51" t="s">
         <v>78</v>
       </c>
@@ -10616,7 +10622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="6" spans="1:3" ht="19.2" customHeight="1">
       <c r="A6" s="51" t="s">
         <v>79</v>
       </c>
@@ -10624,7 +10630,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="7" spans="1:3" ht="19.2" customHeight="1">
       <c r="A7" s="51" t="s">
         <v>80</v>
       </c>
@@ -10635,7 +10641,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="8" spans="1:3" ht="19.2" customHeight="1">
       <c r="A8" s="51" t="s">
         <v>82</v>
       </c>
@@ -10643,7 +10649,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.149999999999999" customHeight="1">
+    <row r="9" spans="1:3" ht="19.2" customHeight="1">
       <c r="A9" s="51" t="s">
         <v>83</v>
       </c>
@@ -10652,6 +10658,17 @@
       </c>
       <c r="C9" s="52" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="43.2">
+      <c r="A10" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="52">
+        <v>5</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -10663,16 +10680,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876A8463-2B96-461E-9F1D-83F4C3412B20}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="1" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -10805,7 +10822,7 @@
         <v>50</v>
       </c>
       <c r="D8">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="E8">
         <v>2032</v>
@@ -10822,7 +10839,7 @@
         <v>50</v>
       </c>
       <c r="D9">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="E9">
         <v>2033</v>
@@ -10839,7 +10856,7 @@
         <v>50</v>
       </c>
       <c r="D10">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="E10">
         <v>2034</v>
@@ -10856,7 +10873,7 @@
         <v>50</v>
       </c>
       <c r="D11">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="E11">
         <v>2035</v>
@@ -10873,7 +10890,7 @@
         <v>50</v>
       </c>
       <c r="D12">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="E12">
         <v>2036</v>
@@ -10890,7 +10907,7 @@
         <v>50</v>
       </c>
       <c r="D13">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="E13">
         <v>2037</v>
@@ -10907,7 +10924,7 @@
         <v>50</v>
       </c>
       <c r="D14">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="E14">
         <v>2038</v>
@@ -10924,7 +10941,7 @@
         <v>50</v>
       </c>
       <c r="D15">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="E15">
         <v>2039</v>
@@ -10941,7 +10958,7 @@
         <v>50</v>
       </c>
       <c r="D16">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="E16">
         <v>2040</v>
@@ -10961,9 +10978,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -10989,7 +11006,7 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:74">
       <c r="A1" s="18" t="s">
@@ -25964,7 +25981,7 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:74">
       <c r="A1" s="18" t="s">
@@ -44983,21 +45000,21 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5703125" customWidth="1"/>
-    <col min="16" max="34" width="26.42578125" customWidth="1"/>
+    <col min="13" max="14" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5546875" customWidth="1"/>
+    <col min="16" max="34" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" customHeight="1">
@@ -47007,23 +47024,23 @@
   <dimension ref="A1:Z974"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="19.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="19.44140625" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -47486,7 +47503,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" s="39" t="s">
         <v>61</v>
@@ -48504,19 +48521,19 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="13" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="5"/>
-    <col min="7" max="7" width="31.28515625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="12.5703125" style="5"/>
+    <col min="6" max="6" width="12.5546875" style="5"/>
+    <col min="7" max="7" width="31.33203125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="12.5546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75">
+    <row r="1" spans="1:7" ht="13.8">
       <c r="A1" s="35" t="s">
         <v>36</v>
       </c>
@@ -48539,7 +48556,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="14.4">
       <c r="A2" s="4">
         <v>0.1</v>
       </c>
@@ -48562,7 +48579,7 @@
         <v>0.7256999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="14.4">
       <c r="A3" s="4">
         <v>0.2</v>
       </c>
@@ -48585,7 +48602,7 @@
         <v>0.77359999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="14.4">
       <c r="A4" s="4">
         <v>0.3</v>
       </c>
@@ -48608,7 +48625,7 @@
         <v>0.78930000000000011</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="14.4">
       <c r="A5" s="4">
         <v>0.4</v>
       </c>
@@ -48631,7 +48648,7 @@
         <v>0.79390000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="14.4">
       <c r="A6" s="4">
         <v>0.5</v>
       </c>
@@ -48654,7 +48671,7 @@
         <v>0.78930000000000011</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="14.4">
       <c r="A7" s="4">
         <v>0.6</v>
       </c>
@@ -48677,7 +48694,7 @@
         <v>0.77839999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="14.4">
       <c r="A8" s="4">
         <v>0.7</v>
       </c>
@@ -48700,7 +48717,7 @@
         <v>0.76659999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="14.4">
       <c r="A9" s="4">
         <v>0.8</v>
       </c>
@@ -48723,7 +48740,7 @@
         <v>0.75450000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="14.4">
       <c r="A10" s="4">
         <v>0.9</v>
       </c>
@@ -48746,7 +48763,7 @@
         <v>0.74219999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="14.4">
       <c r="A11" s="4">
         <v>1</v>
       </c>

</xml_diff>